<commit_message>
Update Template - Projeto de Casos de teste.xlsx
</commit_message>
<xml_diff>
--- a/Template - Projeto de Casos de teste.xlsx
+++ b/Template - Projeto de Casos de teste.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>Quantidade de Argumentos</t>
   </si>
@@ -39,12 +39,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>{0,1,2}</t>
   </si>
   <si>
@@ -123,54 +117,27 @@
     <t>1,3,5,7,8,10,12/Qualquer ano</t>
   </si>
   <si>
-    <t>31 dias</t>
-  </si>
-  <si>
     <t>4,6,9,11/qualquer ano</t>
   </si>
   <si>
-    <t>30 dias</t>
-  </si>
-  <si>
     <t>2/ano bissexto</t>
   </si>
   <si>
-    <t>29 dias</t>
-  </si>
-  <si>
     <t>2/ano não bissexto</t>
   </si>
   <si>
-    <t>28 dias</t>
-  </si>
-  <si>
     <t>Mês I/ ano V</t>
   </si>
   <si>
-    <t>Mensagem de erro mês invalido</t>
-  </si>
-  <si>
     <t>Mês V/Ano I</t>
   </si>
   <si>
-    <t>Mensagem de erro ano inválido</t>
-  </si>
-  <si>
     <t>mês I/ Ano I</t>
   </si>
   <si>
-    <t>Mesagem de erro tudo inválido</t>
-  </si>
-  <si>
     <t xml:space="preserve"> mais de dois argumentos</t>
   </si>
   <si>
-    <t>mensagem erro</t>
-  </si>
-  <si>
-    <t>Mensagem de ano inválido</t>
-  </si>
-  <si>
     <t>CT</t>
   </si>
   <si>
@@ -181,6 +148,117 @@
   </si>
   <si>
     <t>Saída esperada</t>
+  </si>
+  <si>
+    <t>Classes de Equivalência Exercitadas</t>
+  </si>
+  <si>
+    <t>V (1)</t>
+  </si>
+  <si>
+    <t>I (2)</t>
+  </si>
+  <si>
+    <t>9 2020</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>I (3)</t>
+  </si>
+  <si>
+    <t>I (4)</t>
+  </si>
+  <si>
+    <t>I (5)</t>
+  </si>
+  <si>
+    <t>V (6)</t>
+  </si>
+  <si>
+    <t>I (7)</t>
+  </si>
+  <si>
+    <t>I (8)</t>
+  </si>
+  <si>
+    <t>I (9)</t>
+  </si>
+  <si>
+    <t>I (10)</t>
+  </si>
+  <si>
+    <t>I (11)</t>
+  </si>
+  <si>
+    <t>I (12)</t>
+  </si>
+  <si>
+    <t>I (13)</t>
+  </si>
+  <si>
+    <t>I (14)</t>
+  </si>
+  <si>
+    <t>I (15)</t>
+  </si>
+  <si>
+    <t>I (16)</t>
+  </si>
+  <si>
+    <t>I (17)</t>
+  </si>
+  <si>
+    <t>I (18)</t>
+  </si>
+  <si>
+    <t>I (19)</t>
+  </si>
+  <si>
+    <t>I (20)</t>
+  </si>
+  <si>
+    <t>I (21)</t>
+  </si>
+  <si>
+    <t>V (22)</t>
+  </si>
+  <si>
+    <t>365 dias (23)</t>
+  </si>
+  <si>
+    <t>366 dias (24)</t>
+  </si>
+  <si>
+    <t>Mensagem de ano inválido (25)</t>
+  </si>
+  <si>
+    <t>31 dias (26)</t>
+  </si>
+  <si>
+    <t>30 dias (27)</t>
+  </si>
+  <si>
+    <t>29 dias (28)</t>
+  </si>
+  <si>
+    <t>28 dias (29)</t>
+  </si>
+  <si>
+    <t>Mensagem de erro mês invalido (30)</t>
+  </si>
+  <si>
+    <t>Mensagem de erro ano inválido (31)</t>
+  </si>
+  <si>
+    <t>Mesagem de erro tudo inválido (32)</t>
+  </si>
+  <si>
+    <t>mensagem erro (33)</t>
+  </si>
+  <si>
+    <t>1, 29</t>
   </si>
 </sst>
 </file>
@@ -513,23 +591,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="9" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="10" width="26.5" customWidth="1"/>
+    <col min="10" max="10" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -537,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
@@ -545,16 +623,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
@@ -562,224 +640,224 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="1">
-        <v>365</v>
+        <v>23</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="I7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="1">
-        <v>366</v>
+        <v>24</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="I18" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="I19" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="I20" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -789,99 +867,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>14</v>
       </c>

</xml_diff>